<commit_message>
add second ita annotations and calculate metrics
</commit_message>
<xml_diff>
--- a/data/tweets.xlsx
+++ b/data/tweets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="433">
   <si>
     <t>index</t>
   </si>
@@ -616,6 +616,12 @@
     <t>Me and zooey drinking alphabetical order’s on facetime with each other</t>
   </si>
   <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>joy</t>
+  </si>
+  <si>
     <t>61</t>
   </si>
   <si>
@@ -623,6 +629,12 @@
   </si>
   <si>
     <t>iPhone Users 🤝 constantly posting screenshot of songs they listen to, to brag.</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>anger</t>
   </si>
   <si>
     <t>62</t>
@@ -645,6 +657,9 @@
 #DisabilityTwitter #ElectricVehicles</t>
   </si>
   <si>
+    <t>optimism</t>
+  </si>
+  <si>
     <t>64</t>
   </si>
   <si>
@@ -654,6 +669,9 @@
     <t>The metaverse just looks ugly. Like if this is the future why does it look like something made in 2006</t>
   </si>
   <si>
+    <t>sadness</t>
+  </si>
+  <si>
     <t>65</t>
   </si>
   <si>
@@ -661,6 +679,9 @@
   </si>
   <si>
     <t>all i want is to be able to play minecraft on my macbook with my xbox controller.</t>
+  </si>
+  <si>
+    <t>neutral</t>
   </si>
   <si>
     <t>66</t>
@@ -2423,874 +2444,1114 @@
       <c r="C62" s="6" t="s">
         <v>188</v>
       </c>
+      <c r="D62" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="4" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>194</v>
+        <v>198</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>197</v>
+        <v>201</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="4" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>200</v>
+        <v>205</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="4" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" s="4" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>206</v>
+        <v>213</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="4" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>209</v>
+        <v>216</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>212</v>
+      <c r="E70" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="4" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>215</v>
+        <v>222</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="4" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>218</v>
+        <v>225</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="4" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>221</v>
+        <v>228</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="4" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>224</v>
+        <v>231</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="4" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>227</v>
+        <v>234</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="4" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>230</v>
+        <v>237</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" s="4" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>233</v>
+        <v>240</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="4" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>236</v>
+        <v>243</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="4" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>239</v>
+        <v>246</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>242</v>
+        <v>249</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="4" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>245</v>
+        <v>252</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="4" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>248</v>
+        <v>255</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="4" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>251</v>
+        <v>258</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="4" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>254</v>
+        <v>261</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="4" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>257</v>
+        <v>264</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
       <c r="A86" s="4" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>260</v>
+        <v>267</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>263</v>
+        <v>270</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="4" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>266</v>
+        <v>273</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>269</v>
+        <v>276</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>272</v>
+        <v>279</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>275</v>
+        <v>282</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>278</v>
+        <v>285</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>281</v>
+        <v>288</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>284</v>
+        <v>291</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>287</v>
+        <v>294</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="4" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>290</v>
+        <v>297</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="4" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>293</v>
+        <v>300</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>296</v>
+        <v>303</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="4" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>299</v>
+        <v>306</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>302</v>
+        <v>309</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="4" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>305</v>
+        <v>312</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="4" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
     </row>
     <row r="116" ht="14.25" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
     </row>
     <row r="117" ht="14.25" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
     </row>
     <row r="118" ht="14.25" customHeight="1">
       <c r="A118" s="4" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
     </row>
     <row r="119" ht="14.25" customHeight="1">
       <c r="A119" s="4" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
     </row>
     <row r="120" ht="14.25" customHeight="1">
       <c r="A120" s="4" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
     </row>
     <row r="121" ht="14.25" customHeight="1">
       <c r="A121" s="4" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
     </row>
     <row r="122" ht="14.25" customHeight="1">
       <c r="A122" s="4" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="123" ht="14.25" customHeight="1">
       <c r="A123" s="4" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
     </row>
     <row r="124" ht="14.25" customHeight="1">
       <c r="A124" s="4" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="125" ht="14.25" customHeight="1">
       <c r="A125" s="4" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
     </row>
     <row r="126" ht="14.25" customHeight="1">
       <c r="A126" s="4" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
     </row>
     <row r="127" ht="14.25" customHeight="1">
       <c r="A127" s="4" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
     </row>
     <row r="128" ht="14.25" customHeight="1">
       <c r="A128" s="4" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="129" ht="14.25" customHeight="1">
       <c r="A129" s="4" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
     </row>
     <row r="130" ht="14.25" customHeight="1">
       <c r="A130" s="4" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
     </row>
     <row r="131" ht="14.25" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
     </row>
     <row r="132" ht="14.25" customHeight="1">
       <c r="A132" s="4" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
     </row>
     <row r="133" ht="14.25" customHeight="1">
       <c r="A133" s="4" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
     </row>
     <row r="134" ht="14.25" customHeight="1">
       <c r="A134" s="4" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
     </row>
     <row r="135" ht="14.25" customHeight="1">
       <c r="A135" s="4" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
     </row>
     <row r="136" ht="14.25" customHeight="1">
       <c r="A136" s="4" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
     </row>
     <row r="137" ht="14.25" customHeight="1">
       <c r="A137" s="4" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
     </row>
     <row r="138" ht="14.25" customHeight="1">
       <c r="A138" s="4" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
     </row>
     <row r="139" ht="14.25" customHeight="1">
       <c r="A139" s="4" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
     </row>
     <row r="140" ht="14.25" customHeight="1">
       <c r="A140" s="4" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
     </row>
     <row r="141" ht="14.25" customHeight="1">
       <c r="A141" s="4" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
     </row>
     <row r="142" ht="14.25" customHeight="1">

</xml_diff>